<commit_message>
Update Glosario DataEducacion 1.xlsx
</commit_message>
<xml_diff>
--- a/Glosario DataEducacion 1.xlsx
+++ b/Glosario DataEducacion 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATA-EDUCACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228E078F-2BAB-449A-A880-A58657A90D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4E8BBE-BF25-4C2D-B6FC-61AF312370E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{17C7F4D8-EEB3-4ED7-B6A1-07BA937DF46F}"/>
   </bookViews>
@@ -594,7 +594,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>